<commit_message>
Basic adaption of layout and navigation
</commit_message>
<xml_diff>
--- a/xlsforms/consumer.xlsx
+++ b/xlsforms/consumer.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="survey" sheetId="1" state="visible" r:id="rId2"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="135" uniqueCount="104">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="141" uniqueCount="108">
   <si>
     <t xml:space="preserve">type</t>
   </si>
@@ -39,7 +39,7 @@
     <t xml:space="preserve">constraint</t>
   </si>
   <si>
-    <t xml:space="preserve">string</t>
+    <t xml:space="preserve">select_one gender</t>
   </si>
   <si>
     <t xml:space="preserve">gender</t>
@@ -48,25 +48,7 @@
     <t xml:space="preserve">Gender</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">select_one </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">age_groups</t>
-    </r>
+    <t xml:space="preserve">select_one age_groups</t>
   </si>
   <si>
     <t xml:space="preserve">age </t>
@@ -84,25 +66,7 @@
     <t xml:space="preserve">Income (Euro)</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">select_one </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">frequency_number</t>
-    </r>
+    <t xml:space="preserve">select_one frequency_number</t>
   </si>
   <si>
     <t xml:space="preserve">big_chain_store</t>
@@ -138,25 +102,7 @@
     <t xml:space="preserve">Main transport</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">select_one </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">frequency_text</t>
-    </r>
+    <t xml:space="preserve">select_one frequency_text</t>
   </si>
   <si>
     <t xml:space="preserve">bio</t>
@@ -180,25 +126,7 @@
     <t xml:space="preserve">Quantity of consumed tap water (in m³)</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">bottled_water_</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">quantity</t>
-    </r>
+    <t xml:space="preserve">bottled_water_quantity</t>
   </si>
   <si>
     <t xml:space="preserve">Quantity of consumed bottled water (in m³)</t>
@@ -244,6 +172,18 @@
   </si>
   <si>
     <t xml:space="preserve">Enter Manually</t>
+  </si>
+  <si>
+    <t xml:space="preserve">male </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Male</t>
+  </si>
+  <si>
+    <t xml:space="preserve">female</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Female</t>
   </si>
   <si>
     <t xml:space="preserve">age_groups</t>
@@ -415,7 +355,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="12">
+  <fonts count="10">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -469,18 +409,6 @@
       <charset val="1"/>
     </font>
     <font>
-      <sz val="10"/>
-      <color rgb="FF000000"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <color rgb="FF000000"/>
-      <name val="Arial"/>
-      <family val="0"/>
-    </font>
-    <font>
       <sz val="12"/>
       <color rgb="FF000000"/>
       <name val="Times New Roman"/>
@@ -550,7 +478,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="15">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -579,34 +507,18 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
     <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -623,7 +535,7 @@
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -706,8 +618,8 @@
   </sheetPr>
   <dimension ref="A1:AMJ32"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="65" zoomScaleNormal="65" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A21" activeCellId="0" sqref="A21"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -764,7 +676,7 @@
       </c>
     </row>
     <row r="4" customFormat="false" ht="23.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A4" s="7" t="s">
+      <c r="A4" s="1" t="s">
         <v>11</v>
       </c>
       <c r="B4" s="1" t="s">
@@ -774,154 +686,132 @@
         <v>13</v>
       </c>
     </row>
-    <row r="5" s="8" customFormat="true" ht="21.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="5" s="7" customFormat="true" ht="21.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="G5" s="4"/>
       <c r="AMJ5" s="0"/>
     </row>
-    <row r="6" s="9" customFormat="true" ht="21.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A6" s="9" t="s">
+    <row r="6" customFormat="false" ht="21.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A6" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="B6" s="9" t="s">
+      <c r="B6" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="C6" s="10" t="s">
+      <c r="C6" s="8" t="s">
         <v>16</v>
       </c>
-      <c r="G6" s="11"/>
-      <c r="AMJ6" s="11"/>
-    </row>
-    <row r="7" s="9" customFormat="true" ht="21.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A7" s="9" t="s">
+    </row>
+    <row r="7" customFormat="false" ht="21.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A7" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="B7" s="9" t="s">
+      <c r="B7" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="C7" s="10" t="s">
+      <c r="C7" s="8" t="s">
         <v>18</v>
       </c>
-      <c r="G7" s="11"/>
-      <c r="AMJ7" s="11"/>
-    </row>
-    <row r="8" s="9" customFormat="true" ht="21.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A8" s="9" t="s">
+    </row>
+    <row r="8" customFormat="false" ht="21.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A8" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="B8" s="9" t="s">
+      <c r="B8" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="C8" s="10" t="s">
+      <c r="C8" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="G8" s="11"/>
-      <c r="AMJ8" s="11"/>
-    </row>
-    <row r="9" s="9" customFormat="true" ht="21.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A9" s="9" t="s">
+    </row>
+    <row r="9" customFormat="false" ht="21.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A9" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="B9" s="9" t="s">
+      <c r="B9" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="C9" s="10" t="s">
+      <c r="C9" s="8" t="s">
         <v>22</v>
       </c>
-      <c r="G9" s="11"/>
-      <c r="AMJ9" s="11"/>
-    </row>
-    <row r="10" s="9" customFormat="true" ht="21.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A10" s="9" t="s">
+    </row>
+    <row r="10" customFormat="false" ht="21.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A10" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="B10" s="9" t="s">
+      <c r="B10" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="C10" s="10" t="s">
+      <c r="C10" s="8" t="s">
         <v>25</v>
       </c>
-      <c r="G10" s="11"/>
-      <c r="AMJ10" s="11"/>
-    </row>
-    <row r="11" s="9" customFormat="true" ht="21.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A11" s="9" t="s">
+    </row>
+    <row r="11" customFormat="false" ht="21.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A11" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="B11" s="9" t="s">
+      <c r="B11" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="C11" s="10" t="s">
+      <c r="C11" s="8" t="s">
         <v>28</v>
       </c>
-      <c r="G11" s="11"/>
-      <c r="AMJ11" s="11"/>
-    </row>
-    <row r="12" s="9" customFormat="true" ht="21.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A12" s="9" t="s">
+    </row>
+    <row r="12" customFormat="false" ht="21.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A12" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="B12" s="9" t="s">
+      <c r="B12" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="C12" s="10" t="s">
+      <c r="C12" s="8" t="s">
         <v>30</v>
       </c>
-      <c r="G12" s="11"/>
-      <c r="AMJ12" s="11"/>
-    </row>
-    <row r="13" s="9" customFormat="true" ht="21.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A13" s="9" t="s">
+    </row>
+    <row r="13" customFormat="false" ht="21.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A13" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="B13" s="9" t="s">
+      <c r="B13" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="C13" s="10" t="s">
+      <c r="C13" s="8" t="s">
         <v>33</v>
       </c>
-      <c r="G13" s="11"/>
-      <c r="AMJ13" s="11"/>
-    </row>
-    <row r="14" s="9" customFormat="true" ht="21.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A14" s="9" t="s">
+    </row>
+    <row r="14" customFormat="false" ht="21.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A14" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="B14" s="9" t="s">
+      <c r="B14" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="C14" s="10" t="s">
+      <c r="C14" s="8" t="s">
         <v>35</v>
       </c>
-      <c r="G14" s="11"/>
-      <c r="AMJ14" s="11"/>
-    </row>
-    <row r="15" s="9" customFormat="true" ht="21.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A15" s="9" t="s">
+    </row>
+    <row r="15" customFormat="false" ht="21.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A15" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="B15" s="9" t="s">
+      <c r="B15" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="C15" s="10" t="s">
+      <c r="C15" s="8" t="s">
         <v>38</v>
       </c>
-      <c r="G15" s="11"/>
-      <c r="AMJ15" s="11"/>
-    </row>
-    <row r="16" s="9" customFormat="true" ht="21.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A16" s="9" t="s">
+    </row>
+    <row r="16" customFormat="false" ht="21.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A16" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="B16" s="12" t="s">
+      <c r="B16" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="C16" s="10" t="s">
+      <c r="C16" s="8" t="s">
         <v>41</v>
       </c>
-      <c r="G16" s="11"/>
-      <c r="AMJ16" s="11"/>
-    </row>
-    <row r="17" s="8" customFormat="true" ht="22.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    </row>
+    <row r="17" s="7" customFormat="true" ht="22.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="G17" s="4"/>
       <c r="AMJ17" s="0"/>
     </row>
@@ -992,27 +882,27 @@
   </sheetPr>
   <dimension ref="A1:D1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="65" zoomScaleNormal="65" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A26" activeCellId="0" sqref="A26"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C6" activeCellId="0" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="13" width="31.12"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="13" width="28.19"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="13" width="81.14"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="13" width="17.64"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="5" style="13" width="14.43"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="9" width="31.12"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="9" width="28.19"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="9" width="81.14"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="9" width="17.64"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="5" style="9" width="14.43"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A1" s="14" t="s">
+      <c r="A1" s="10" t="s">
         <v>42</v>
       </c>
-      <c r="B1" s="14" t="s">
+      <c r="B1" s="10" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="15" t="s">
+      <c r="C1" s="11" t="s">
         <v>2</v>
       </c>
     </row>
@@ -1054,29 +944,31 @@
     </row>
     <row r="5" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A5" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B5" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="B5" s="1" t="s">
+      <c r="C5" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="C5" s="0" t="s">
-        <v>52</v>
-      </c>
+      <c r="D5" s="0"/>
     </row>
     <row r="6" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A6" s="1" t="s">
-        <v>50</v>
+        <v>6</v>
       </c>
       <c r="B6" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="C6" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="C6" s="0" t="s">
-        <v>54</v>
-      </c>
+      <c r="D6" s="0"/>
     </row>
     <row r="7" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A7" s="1" t="s">
-        <v>50</v>
+        <v>54</v>
       </c>
       <c r="B7" s="1" t="s">
         <v>55</v>
@@ -1087,7 +979,7 @@
     </row>
     <row r="8" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A8" s="1" t="s">
-        <v>50</v>
+        <v>54</v>
       </c>
       <c r="B8" s="1" t="s">
         <v>57</v>
@@ -1098,7 +990,7 @@
     </row>
     <row r="9" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A9" s="1" t="s">
-        <v>12</v>
+        <v>54</v>
       </c>
       <c r="B9" s="1" t="s">
         <v>59</v>
@@ -1107,9 +999,9 @@
         <v>60</v>
       </c>
     </row>
-    <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="10" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A10" s="1" t="s">
-        <v>12</v>
+        <v>54</v>
       </c>
       <c r="B10" s="1" t="s">
         <v>61</v>
@@ -1118,7 +1010,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="11" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A11" s="1" t="s">
         <v>12</v>
       </c>
@@ -1131,56 +1023,56 @@
     </row>
     <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B12" s="1" t="s">
         <v>65</v>
       </c>
-      <c r="B12" s="16" t="n">
-        <v>1</v>
-      </c>
-      <c r="C12" s="17" t="n">
-        <v>1</v>
+      <c r="C12" s="0" t="s">
+        <v>66</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="1" t="s">
-        <v>65</v>
-      </c>
-      <c r="B13" s="16" t="n">
+        <v>12</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="C13" s="0" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="B14" s="12" t="n">
+        <v>1</v>
+      </c>
+      <c r="C14" s="13" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="B15" s="12" t="n">
         <v>3</v>
       </c>
-      <c r="C13" s="0" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="14" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A14" s="1" t="s">
-        <v>65</v>
-      </c>
-      <c r="B14" s="1" t="s">
-        <v>67</v>
-      </c>
-      <c r="C14" s="0" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="15" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A15" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="B15" s="1" t="s">
-        <v>69</v>
-      </c>
-      <c r="C15" s="1" t="s">
+      <c r="C15" s="0" t="s">
         <v>70</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A16" s="1" t="s">
-        <v>24</v>
+        <v>69</v>
       </c>
       <c r="B16" s="1" t="s">
         <v>71</v>
       </c>
-      <c r="C16" s="1" t="s">
+      <c r="C16" s="0" t="s">
         <v>72</v>
       </c>
     </row>
@@ -1202,46 +1094,46 @@
       <c r="B18" s="1" t="s">
         <v>75</v>
       </c>
-      <c r="C18" s="0" t="s">
+      <c r="C18" s="1" t="s">
         <v>76</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A19" s="7" t="s">
+      <c r="A19" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="B19" s="1" t="s">
         <v>77</v>
       </c>
-      <c r="B19" s="1" t="s">
+      <c r="C19" s="1" t="s">
         <v>78</v>
       </c>
-      <c r="C19" s="1" t="s">
+    </row>
+    <row r="20" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A20" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="B20" s="1" t="s">
         <v>79</v>
       </c>
-    </row>
-    <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="7" t="s">
-        <v>77</v>
-      </c>
-      <c r="B20" s="1" t="s">
+      <c r="C20" s="0" t="s">
         <v>80</v>
       </c>
-      <c r="C20" s="1" t="s">
+    </row>
+    <row r="21" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A21" s="1" t="s">
         <v>81</v>
-      </c>
-    </row>
-    <row r="21" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A21" s="7" t="s">
-        <v>77</v>
       </c>
       <c r="B21" s="1" t="s">
         <v>82</v>
       </c>
-      <c r="C21" s="0" t="s">
+      <c r="C21" s="1" t="s">
         <v>83</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="1" t="s">
-        <v>40</v>
+        <v>81</v>
       </c>
       <c r="B22" s="1" t="s">
         <v>84</v>
@@ -1252,12 +1144,12 @@
     </row>
     <row r="23" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="1" t="s">
-        <v>40</v>
+        <v>81</v>
       </c>
       <c r="B23" s="1" t="s">
         <v>86</v>
       </c>
-      <c r="C23" s="1" t="s">
+      <c r="C23" s="0" t="s">
         <v>87</v>
       </c>
     </row>
@@ -1279,13 +1171,13 @@
       <c r="B25" s="1" t="s">
         <v>90</v>
       </c>
-      <c r="C25" s="0" t="s">
+      <c r="C25" s="1" t="s">
         <v>91</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="1" t="s">
-        <v>37</v>
+        <v>40</v>
       </c>
       <c r="B26" s="1" t="s">
         <v>92</v>
@@ -1296,12 +1188,12 @@
     </row>
     <row r="27" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="1" t="s">
-        <v>37</v>
+        <v>40</v>
       </c>
       <c r="B27" s="1" t="s">
         <v>94</v>
       </c>
-      <c r="C27" s="1" t="s">
+      <c r="C27" s="0" t="s">
         <v>95</v>
       </c>
     </row>
@@ -1316,8 +1208,28 @@
         <v>97</v>
       </c>
     </row>
-    <row r="1048573" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048574" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="29" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A29" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="B29" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="C29" s="1" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="30" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A30" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="B30" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="C30" s="1" t="s">
+        <v>101</v>
+      </c>
+    </row>
     <row r="1048575" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
@@ -1338,7 +1250,7 @@
   </sheetPr>
   <dimension ref="A1:E5"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="65" zoomScaleNormal="65" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="C2" activeCellId="0" sqref="C2"/>
     </sheetView>
   </sheetViews>
@@ -1353,34 +1265,34 @@
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A1" s="14" t="s">
-        <v>98</v>
-      </c>
-      <c r="B1" s="14" t="s">
-        <v>99</v>
-      </c>
-      <c r="C1" s="14" t="s">
-        <v>100</v>
-      </c>
-      <c r="D1" s="15" t="s">
-        <v>101</v>
-      </c>
-      <c r="E1" s="15" t="s">
+      <c r="A1" s="10" t="s">
         <v>102</v>
       </c>
+      <c r="B1" s="10" t="s">
+        <v>103</v>
+      </c>
+      <c r="C1" s="10" t="s">
+        <v>104</v>
+      </c>
+      <c r="D1" s="11" t="s">
+        <v>105</v>
+      </c>
+      <c r="E1" s="11" t="s">
+        <v>106</v>
+      </c>
     </row>
     <row r="2" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A2" s="18" t="s">
-        <v>103</v>
-      </c>
-      <c r="B2" s="18"/>
-      <c r="C2" s="18" t="s">
-        <v>103</v>
-      </c>
-      <c r="D2" s="18" t="n">
+      <c r="A2" s="14" t="s">
+        <v>107</v>
+      </c>
+      <c r="B2" s="14"/>
+      <c r="C2" s="14" t="s">
+        <v>107</v>
+      </c>
+      <c r="D2" s="14" t="n">
         <v>1</v>
       </c>
-      <c r="E2" s="18"/>
+      <c r="E2" s="14"/>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>

</xml_diff>